<commit_message>
Added heat maps and updated the visualisations
</commit_message>
<xml_diff>
--- a/merged_cells_testing.xlsx
+++ b/merged_cells_testing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\spreadsheet-analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644D1BBE-B634-4D14-AB27-08C87D8D9383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E13AF5A-F3E1-4340-89C8-787E5B3ED0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4305" yWindow="3675" windowWidth="21600" windowHeight="10710" xr2:uid="{D4764ED0-F097-4F39-83A4-67F9EFBA64E8}"/>
+    <workbookView xWindow="32445" yWindow="1470" windowWidth="21600" windowHeight="12270" xr2:uid="{D4764ED0-F097-4F39-83A4-67F9EFBA64E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,15 +388,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFD079E-09C2-458F-9700-199722C7742F}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F7:F8"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,12 +404,14 @@
         <v>1</v>
       </c>
       <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>